<commit_message>
Padam paatam edit Templates 01/01/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 3.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 3.3 Padam Input Template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5041" uniqueCount="1282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5074" uniqueCount="1292">
   <si>
     <t>PS</t>
   </si>
@@ -3873,6 +3873,36 @@
   </si>
   <si>
     <t>Kampam</t>
+  </si>
+  <si>
+    <t>P[r]+N[r]</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>ngg</t>
+  </si>
+  <si>
+    <t>S[s]</t>
+  </si>
+  <si>
+    <t>RE+SE</t>
+  </si>
+  <si>
+    <t>RE</t>
+  </si>
+  <si>
+    <t>SE+RE</t>
+  </si>
+  <si>
+    <t>NSE+NRE</t>
+  </si>
+  <si>
+    <t>NSE</t>
+  </si>
+  <si>
+    <t>S[Sh]</t>
   </si>
 </sst>
 </file>
@@ -4006,7 +4036,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4022,6 +4052,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4053,7 +4095,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4218,6 +4260,68 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4501,10 +4605,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V1858"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1733" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1374" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="A702" sqref="A702"/>
+      <selection pane="bottomLeft" activeCell="N1383" sqref="N1383"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -4520,7 +4624,7 @@
     <col min="11" max="11" width="13.5703125" style="18" customWidth="1"/>
     <col min="12" max="12" width="15.28515625" style="5" customWidth="1"/>
     <col min="13" max="13" width="18.140625" style="5" customWidth="1"/>
-    <col min="14" max="14" width="79.7109375" style="4" customWidth="1"/>
+    <col min="14" max="14" width="37.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7.7109375" style="3" customWidth="1"/>
     <col min="16" max="17" width="5.7109375" style="1" customWidth="1"/>
     <col min="18" max="18" width="6.28515625" style="1" customWidth="1"/>
@@ -8433,8 +8537,12 @@
       <c r="P89" s="11"/>
       <c r="Q89" s="11"/>
       <c r="R89" s="11"/>
-      <c r="S89" s="11"/>
-      <c r="T89" s="11"/>
+      <c r="S89" s="11" t="s">
+        <v>1253</v>
+      </c>
+      <c r="T89" s="11" t="s">
+        <v>1282</v>
+      </c>
       <c r="U89" s="11"/>
       <c r="V89" s="46"/>
     </row>
@@ -8659,8 +8767,12 @@
       <c r="P95" s="7"/>
       <c r="Q95" s="7"/>
       <c r="R95" s="7"/>
-      <c r="S95" s="7"/>
-      <c r="T95" s="7"/>
+      <c r="S95" s="11" t="s">
+        <v>1253</v>
+      </c>
+      <c r="T95" s="11" t="s">
+        <v>1282</v>
+      </c>
       <c r="U95" s="7"/>
       <c r="V95" s="46"/>
     </row>
@@ -8813,8 +8925,12 @@
       <c r="P99" s="7"/>
       <c r="Q99" s="7"/>
       <c r="R99" s="7"/>
-      <c r="S99" s="7"/>
-      <c r="T99" s="7"/>
+      <c r="S99" s="11" t="s">
+        <v>1253</v>
+      </c>
+      <c r="T99" s="11" t="s">
+        <v>1282</v>
+      </c>
       <c r="U99" s="7"/>
       <c r="V99" s="46"/>
     </row>
@@ -16596,7 +16712,9 @@
       <c r="R305" s="7"/>
       <c r="S305" s="7"/>
       <c r="T305" s="7"/>
-      <c r="U305" s="7"/>
+      <c r="U305" s="7" t="s">
+        <v>1283</v>
+      </c>
       <c r="V305" s="46"/>
     </row>
     <row r="306" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -17017,7 +17135,9 @@
       <c r="R316" s="7"/>
       <c r="S316" s="7"/>
       <c r="T316" s="7"/>
-      <c r="U316" s="7"/>
+      <c r="U316" s="7" t="s">
+        <v>1283</v>
+      </c>
       <c r="V316" s="46"/>
     </row>
     <row r="317" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -17477,7 +17597,9 @@
       <c r="R328" s="7"/>
       <c r="S328" s="7"/>
       <c r="T328" s="7"/>
-      <c r="U328" s="7"/>
+      <c r="U328" s="7" t="s">
+        <v>1283</v>
+      </c>
       <c r="V328" s="46"/>
     </row>
     <row r="329" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -21210,42 +21332,42 @@
       <c r="U426" s="7"/>
       <c r="V426" s="46"/>
     </row>
-    <row r="427" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A427" s="7"/>
-      <c r="D427" s="26"/>
-      <c r="E427" s="20"/>
-      <c r="F427" s="20"/>
-      <c r="G427" s="20"/>
-      <c r="H427" s="20"/>
-      <c r="I427" s="45" t="s">
+    <row r="427" spans="1:22" s="58" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A427" s="57"/>
+      <c r="D427" s="59"/>
+      <c r="E427" s="60"/>
+      <c r="F427" s="60"/>
+      <c r="G427" s="60"/>
+      <c r="H427" s="60"/>
+      <c r="I427" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="J427" s="9">
+      <c r="J427" s="62">
         <v>8</v>
       </c>
-      <c r="K427" s="17">
+      <c r="K427" s="63">
         <f t="shared" si="18"/>
         <v>426</v>
       </c>
-      <c r="L427" s="17">
+      <c r="L427" s="63">
         <f t="shared" si="19"/>
         <v>50</v>
       </c>
-      <c r="M427" s="17">
+      <c r="M427" s="63">
         <f t="shared" si="20"/>
         <v>50</v>
       </c>
-      <c r="N427" s="46" t="s">
+      <c r="N427" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="O427" s="6"/>
-      <c r="P427" s="7"/>
-      <c r="Q427" s="7"/>
-      <c r="R427" s="7"/>
-      <c r="S427" s="7"/>
-      <c r="T427" s="7"/>
-      <c r="U427" s="7"/>
-      <c r="V427" s="46"/>
+      <c r="O427" s="65"/>
+      <c r="P427" s="57"/>
+      <c r="Q427" s="57"/>
+      <c r="R427" s="57"/>
+      <c r="S427" s="57"/>
+      <c r="T427" s="57"/>
+      <c r="U427" s="57"/>
+      <c r="V427" s="64"/>
     </row>
     <row r="428" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A428" s="7"/>
@@ -22915,7 +23037,9 @@
       <c r="P472" s="7"/>
       <c r="Q472" s="7"/>
       <c r="R472" s="7"/>
-      <c r="S472" s="7"/>
+      <c r="S472" s="7" t="s">
+        <v>1266</v>
+      </c>
       <c r="T472" s="7"/>
       <c r="U472" s="7"/>
       <c r="V472" s="46"/>
@@ -33639,8 +33763,12 @@
       <c r="P761" s="7"/>
       <c r="Q761" s="7"/>
       <c r="R761" s="7"/>
-      <c r="S761" s="7"/>
-      <c r="T761" s="7"/>
+      <c r="S761" s="7" t="s">
+        <v>1284</v>
+      </c>
+      <c r="T761" s="7" t="s">
+        <v>1285</v>
+      </c>
       <c r="U761" s="7"/>
       <c r="V761" s="46"/>
     </row>
@@ -36085,7 +36213,9 @@
       <c r="R829" s="7"/>
       <c r="S829" s="7"/>
       <c r="T829" s="7"/>
-      <c r="U829" s="7"/>
+      <c r="U829" s="7" t="s">
+        <v>1286</v>
+      </c>
       <c r="V829" s="46"/>
     </row>
     <row r="830" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36332,8 +36462,10 @@
       <c r="P836" s="7"/>
       <c r="Q836" s="7"/>
       <c r="R836" s="7"/>
-      <c r="S836" s="7"/>
-      <c r="T836" s="7"/>
+      <c r="S836" s="7" t="s">
+        <v>1253</v>
+      </c>
+      <c r="T836" s="66"/>
       <c r="U836" s="7"/>
       <c r="V836" s="46"/>
     </row>
@@ -36550,7 +36682,9 @@
       <c r="R842" s="7"/>
       <c r="S842" s="7"/>
       <c r="T842" s="7"/>
-      <c r="U842" s="7"/>
+      <c r="U842" s="7" t="s">
+        <v>1287</v>
+      </c>
       <c r="V842" s="46" t="s">
         <v>414</v>
       </c>
@@ -37298,7 +37432,9 @@
       <c r="R863" s="7"/>
       <c r="S863" s="7"/>
       <c r="T863" s="7"/>
-      <c r="U863" s="7"/>
+      <c r="U863" s="7" t="s">
+        <v>1276</v>
+      </c>
       <c r="V863" s="46" t="s">
         <v>429</v>
       </c>
@@ -37623,7 +37759,9 @@
       <c r="R872" s="7"/>
       <c r="S872" s="7"/>
       <c r="T872" s="7"/>
-      <c r="U872" s="7"/>
+      <c r="U872" s="7" t="s">
+        <v>1288</v>
+      </c>
       <c r="V872" s="46" t="s">
         <v>436</v>
       </c>
@@ -39439,8 +39577,12 @@
       <c r="P922" s="7"/>
       <c r="Q922" s="7"/>
       <c r="R922" s="7"/>
-      <c r="S922" s="7"/>
-      <c r="T922" s="7"/>
+      <c r="S922" s="7" t="s">
+        <v>1237</v>
+      </c>
+      <c r="T922" s="7" t="s">
+        <v>1237</v>
+      </c>
       <c r="U922" s="7"/>
       <c r="V922" s="46"/>
     </row>
@@ -45276,7 +45418,9 @@
       <c r="R1084" s="7"/>
       <c r="S1084" s="7"/>
       <c r="T1084" s="7"/>
-      <c r="U1084" s="7"/>
+      <c r="U1084" s="7" t="s">
+        <v>1289</v>
+      </c>
       <c r="V1084" s="46"/>
     </row>
     <row r="1085" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46481,7 +46625,9 @@
       <c r="R1115" s="7"/>
       <c r="S1115" s="7"/>
       <c r="T1115" s="7"/>
-      <c r="U1115" s="7"/>
+      <c r="U1115" s="7" t="s">
+        <v>1289</v>
+      </c>
       <c r="V1115" s="46"/>
     </row>
     <row r="1116" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48563,7 +48709,9 @@
       <c r="R1172" s="7"/>
       <c r="S1172" s="7"/>
       <c r="T1172" s="7"/>
-      <c r="U1172" s="7"/>
+      <c r="U1172" s="7" t="s">
+        <v>1283</v>
+      </c>
       <c r="V1172" s="46"/>
     </row>
     <row r="1173" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48957,8 +49105,12 @@
       <c r="P1183" s="7"/>
       <c r="Q1183" s="7"/>
       <c r="R1183" s="7"/>
-      <c r="S1183" s="7"/>
-      <c r="T1183" s="7"/>
+      <c r="S1183" s="7" t="s">
+        <v>1253</v>
+      </c>
+      <c r="T1183" s="7" t="s">
+        <v>1259</v>
+      </c>
       <c r="U1183" s="7"/>
       <c r="V1183" s="46"/>
     </row>
@@ -51392,7 +51544,9 @@
       <c r="R1249" s="7"/>
       <c r="S1249" s="7"/>
       <c r="T1249" s="7"/>
-      <c r="U1249" s="7"/>
+      <c r="U1249" s="7" t="s">
+        <v>1290</v>
+      </c>
       <c r="V1249" s="46"/>
     </row>
     <row r="1250" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53948,8 +54102,12 @@
       <c r="P1319" s="7"/>
       <c r="Q1319" s="7"/>
       <c r="R1319" s="7"/>
-      <c r="S1319" s="7"/>
-      <c r="T1319" s="7"/>
+      <c r="S1319" s="7" t="s">
+        <v>1284</v>
+      </c>
+      <c r="T1319" s="7" t="s">
+        <v>1285</v>
+      </c>
       <c r="U1319" s="7"/>
       <c r="V1319" s="46"/>
     </row>
@@ -55082,8 +55240,12 @@
       <c r="P1350" s="7"/>
       <c r="Q1350" s="7"/>
       <c r="R1350" s="7"/>
-      <c r="S1350" s="7"/>
-      <c r="T1350" s="7"/>
+      <c r="S1350" s="7" t="s">
+        <v>1253</v>
+      </c>
+      <c r="T1350" s="7" t="s">
+        <v>1259</v>
+      </c>
       <c r="U1350" s="7"/>
       <c r="V1350" s="46"/>
     </row>
@@ -55298,8 +55460,12 @@
       <c r="P1356" s="7"/>
       <c r="Q1356" s="7"/>
       <c r="R1356" s="7"/>
-      <c r="S1356" s="7"/>
-      <c r="T1356" s="7"/>
+      <c r="S1356" s="7" t="s">
+        <v>1253</v>
+      </c>
+      <c r="T1356" s="7" t="s">
+        <v>1259</v>
+      </c>
       <c r="U1356" s="7"/>
       <c r="V1356" s="46"/>
     </row>
@@ -55334,8 +55500,12 @@
       <c r="P1357" s="7"/>
       <c r="Q1357" s="7"/>
       <c r="R1357" s="7"/>
-      <c r="S1357" s="7"/>
-      <c r="T1357" s="7"/>
+      <c r="S1357" s="7" t="s">
+        <v>1253</v>
+      </c>
+      <c r="T1357" s="7" t="s">
+        <v>1291</v>
+      </c>
       <c r="U1357" s="7"/>
       <c r="V1357" s="46"/>
     </row>
@@ -56030,7 +56200,7 @@
       <c r="U1376" s="7"/>
       <c r="V1376" s="46"/>
     </row>
-    <row r="1377" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1377" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1377" s="44"/>
       <c r="E1377" s="20"/>
       <c r="F1377" s="20"/>
@@ -56066,7 +56236,7 @@
       <c r="U1377" s="7"/>
       <c r="V1377" s="46"/>
     </row>
-    <row r="1378" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1378" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1378" s="44"/>
       <c r="E1378" s="20"/>
       <c r="F1378" s="20"/>
@@ -56102,7 +56272,7 @@
       <c r="U1378" s="7"/>
       <c r="V1378" s="46"/>
     </row>
-    <row r="1379" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1379" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1379" s="44"/>
       <c r="E1379" s="20"/>
       <c r="F1379" s="20"/>
@@ -56138,7 +56308,7 @@
       <c r="U1379" s="7"/>
       <c r="V1379" s="46"/>
     </row>
-    <row r="1380" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1380" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1380" s="44"/>
       <c r="E1380" s="20"/>
       <c r="F1380" s="20"/>
@@ -56174,7 +56344,7 @@
       <c r="U1380" s="7"/>
       <c r="V1380" s="46"/>
     </row>
-    <row r="1381" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1381" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1381" s="44"/>
       <c r="E1381" s="20"/>
       <c r="F1381" s="20"/>
@@ -56210,47 +56380,49 @@
       <c r="U1381" s="7"/>
       <c r="V1381" s="46"/>
     </row>
-    <row r="1382" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="C1382" s="44"/>
-      <c r="E1382" s="20"/>
-      <c r="F1382" s="20"/>
-      <c r="G1382" s="20"/>
-      <c r="H1382" s="39"/>
-      <c r="I1382" s="45" t="s">
+    <row r="1382" spans="1:22" s="69" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A1382" s="68"/>
+      <c r="C1382" s="70"/>
+      <c r="D1382" s="71"/>
+      <c r="E1382" s="72"/>
+      <c r="F1382" s="72"/>
+      <c r="G1382" s="72"/>
+      <c r="H1382" s="73"/>
+      <c r="I1382" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="J1382" s="9">
+      <c r="J1382" s="75">
         <v>27</v>
       </c>
-      <c r="K1382" s="17">
+      <c r="K1382" s="76">
         <f t="shared" si="63"/>
         <v>1381</v>
       </c>
-      <c r="L1382" s="17">
+      <c r="L1382" s="76">
         <f t="shared" si="64"/>
         <v>50</v>
       </c>
-      <c r="M1382" s="17">
+      <c r="M1382" s="76">
         <f t="shared" si="65"/>
         <v>300</v>
       </c>
-      <c r="N1382" s="46" t="s">
+      <c r="N1382" s="77" t="s">
         <v>658</v>
       </c>
-      <c r="O1382" s="6"/>
-      <c r="P1382" s="7" t="s">
+      <c r="O1382" s="78"/>
+      <c r="P1382" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="Q1382" s="7"/>
-      <c r="R1382" s="7"/>
-      <c r="S1382" s="7"/>
-      <c r="T1382" s="7"/>
-      <c r="U1382" s="7"/>
-      <c r="V1382" s="46" t="s">
+      <c r="Q1382" s="67"/>
+      <c r="R1382" s="67"/>
+      <c r="S1382" s="67"/>
+      <c r="T1382" s="67"/>
+      <c r="U1382" s="67"/>
+      <c r="V1382" s="77" t="s">
         <v>1187</v>
       </c>
     </row>
-    <row r="1383" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1383" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1383" s="44"/>
       <c r="E1383" s="20"/>
       <c r="F1383" s="20"/>
@@ -56284,7 +56456,7 @@
       <c r="U1383" s="7"/>
       <c r="V1383" s="46"/>
     </row>
-    <row r="1384" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1384" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1384" s="44"/>
       <c r="E1384" s="20"/>
       <c r="F1384" s="20"/>
@@ -56320,7 +56492,7 @@
       <c r="U1384" s="7"/>
       <c r="V1384" s="46"/>
     </row>
-    <row r="1385" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1385" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1385" s="44"/>
       <c r="E1385" s="20"/>
       <c r="F1385" s="20"/>
@@ -56358,7 +56530,7 @@
       <c r="U1385" s="7"/>
       <c r="V1385" s="46"/>
     </row>
-    <row r="1386" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1386" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1386" s="44"/>
       <c r="E1386" s="20"/>
       <c r="F1386" s="20"/>
@@ -56394,7 +56566,7 @@
       <c r="U1386" s="7"/>
       <c r="V1386" s="46"/>
     </row>
-    <row r="1387" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1387" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1387" s="44"/>
       <c r="E1387" s="20"/>
       <c r="F1387" s="20"/>
@@ -56430,7 +56602,7 @@
       <c r="U1387" s="7"/>
       <c r="V1387" s="46"/>
     </row>
-    <row r="1388" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1388" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1388" s="44"/>
       <c r="E1388" s="20"/>
       <c r="F1388" s="20"/>
@@ -56466,7 +56638,7 @@
       <c r="U1388" s="7"/>
       <c r="V1388" s="46"/>
     </row>
-    <row r="1389" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1389" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1389" s="44"/>
       <c r="E1389" s="20"/>
       <c r="F1389" s="20"/>
@@ -56502,7 +56674,7 @@
       <c r="U1389" s="7"/>
       <c r="V1389" s="46"/>
     </row>
-    <row r="1390" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1390" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1390" s="44"/>
       <c r="E1390" s="20"/>
       <c r="F1390" s="20"/>
@@ -56538,7 +56710,7 @@
       <c r="U1390" s="7"/>
       <c r="V1390" s="46"/>
     </row>
-    <row r="1391" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1391" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1391" s="44"/>
       <c r="E1391" s="20"/>
       <c r="F1391" s="20"/>
@@ -56578,7 +56750,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="1392" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1392" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1392" s="44"/>
       <c r="E1392" s="20"/>
       <c r="F1392" s="20"/>

</xml_diff>

<commit_message>
TS Padam Templates and TTD 02/01/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 3.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 3.3 Padam Input Template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5074" uniqueCount="1292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5091" uniqueCount="1294">
   <si>
     <t>PS</t>
   </si>
@@ -3903,6 +3903,12 @@
   </si>
   <si>
     <t>S[Sh]</t>
+  </si>
+  <si>
+    <t>NE+NRE</t>
+  </si>
+  <si>
+    <t>NE+NSE+NRE</t>
   </si>
 </sst>
 </file>
@@ -4606,9 +4612,9 @@
   <dimension ref="A1:V1858"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1374" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1848" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N1383" sqref="N1383"/>
+      <selection pane="bottomLeft" activeCell="U1848" sqref="U1848"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -56965,8 +56971,12 @@
       <c r="P1397" s="7"/>
       <c r="Q1397" s="7"/>
       <c r="R1397" s="7"/>
-      <c r="S1397" s="7"/>
-      <c r="T1397" s="7"/>
+      <c r="S1397" s="7" t="s">
+        <v>1253</v>
+      </c>
+      <c r="T1397" s="7" t="s">
+        <v>1259</v>
+      </c>
       <c r="U1397" s="7"/>
       <c r="V1397" s="46"/>
     </row>
@@ -58560,8 +58570,12 @@
       <c r="P1440" s="7"/>
       <c r="Q1440" s="7"/>
       <c r="R1440" s="7"/>
-      <c r="S1440" s="7"/>
-      <c r="T1440" s="7"/>
+      <c r="S1440" s="7" t="s">
+        <v>1253</v>
+      </c>
+      <c r="T1440" s="7" t="s">
+        <v>1291</v>
+      </c>
       <c r="U1440" s="7"/>
       <c r="V1440" s="46"/>
     </row>
@@ -62730,7 +62744,9 @@
       <c r="R1552" s="7"/>
       <c r="S1552" s="7"/>
       <c r="T1552" s="7"/>
-      <c r="U1552" s="7"/>
+      <c r="U1552" s="7" t="s">
+        <v>1283</v>
+      </c>
       <c r="V1552" s="46"/>
     </row>
     <row r="1553" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65304,6 +65320,9 @@
       <c r="N1633" s="46" t="s">
         <v>514</v>
       </c>
+      <c r="U1633" s="1" t="s">
+        <v>1293</v>
+      </c>
       <c r="V1633" s="46"/>
     </row>
     <row r="1634" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65669,6 +65688,9 @@
       <c r="N1646" s="46" t="s">
         <v>514</v>
       </c>
+      <c r="U1646" s="1" t="s">
+        <v>1290</v>
+      </c>
       <c r="V1646" s="46"/>
     </row>
     <row r="1647" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66223,6 +66245,12 @@
       <c r="N1665" s="46" t="s">
         <v>837</v>
       </c>
+      <c r="S1665" s="1" t="s">
+        <v>1253</v>
+      </c>
+      <c r="T1665" s="1" t="s">
+        <v>1259</v>
+      </c>
       <c r="V1665" s="46"/>
     </row>
     <row r="1666" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66253,6 +66281,12 @@
       <c r="P1666" s="7" t="s">
         <v>19</v>
       </c>
+      <c r="S1666" s="1" t="s">
+        <v>1253</v>
+      </c>
+      <c r="T1666" s="1" t="s">
+        <v>1291</v>
+      </c>
       <c r="V1666" s="46" t="s">
         <v>1213</v>
       </c>
@@ -70055,6 +70089,9 @@
       <c r="N1796" s="46" t="s">
         <v>912</v>
       </c>
+      <c r="U1796" s="1" t="s">
+        <v>1290</v>
+      </c>
       <c r="V1796" s="46"/>
     </row>
     <row r="1797" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70566,6 +70603,9 @@
       <c r="N1814" s="46" t="s">
         <v>868</v>
       </c>
+      <c r="U1814" s="1" t="s">
+        <v>1283</v>
+      </c>
       <c r="V1814" s="46"/>
     </row>
     <row r="1815" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70969,6 +71009,9 @@
       <c r="N1827" s="46" t="s">
         <v>936</v>
       </c>
+      <c r="U1827" s="1" t="s">
+        <v>1258</v>
+      </c>
       <c r="V1827" s="46"/>
     </row>
     <row r="1828" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71527,6 +71570,9 @@
       <c r="N1847" s="46" t="s">
         <v>946</v>
       </c>
+      <c r="U1847" s="1" t="s">
+        <v>1292</v>
+      </c>
       <c r="V1847" s="46"/>
     </row>
     <row r="1848" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71750,6 +71796,12 @@
       </c>
       <c r="N1855" s="46" t="s">
         <v>590</v>
+      </c>
+      <c r="S1855" s="1" t="s">
+        <v>1253</v>
+      </c>
+      <c r="T1855" s="1" t="s">
+        <v>1259</v>
       </c>
       <c r="V1855" s="46"/>
     </row>

</xml_diff>